<commit_message>
add 1k test data generation script
</commit_message>
<xml_diff>
--- a/doc/TopN time estimation.xlsx
+++ b/doc/TopN time estimation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>n</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Dec</t>
+  </si>
+  <si>
+    <t>891 test, 51 nonzero</t>
   </si>
 </sst>
 </file>
@@ -548,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,6 +903,21 @@
       </c>
       <c r="K15">
         <v>2.9762499999999998</v>
+      </c>
+      <c r="N15">
+        <v>74.17</v>
+      </c>
+      <c r="O15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0.72</v>
+      </c>
+      <c r="R15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>